<commit_message>
Added serial run capture data
</commit_message>
<xml_diff>
--- a/docs/Test Results; 2011-04.xlsx
+++ b/docs/Test Results; 2011-04.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="42">
   <si>
     <t>Tester</t>
   </si>
@@ -129,6 +129,18 @@
   </si>
   <si>
     <t>Dist Cow - Average Run time milliseconds (no clock sync to master)</t>
+  </si>
+  <si>
+    <t>Serial</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>N/A - cmdline = time cowpatty -d, -r, -s</t>
+  </si>
+  <si>
+    <t>Serial coWPAtty run time (milliseconds)</t>
   </si>
 </sst>
 </file>
@@ -136,10 +148,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="172" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="173" formatCode="[h]:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +163,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -176,13 +195,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -491,11 +511,12 @@
     <col min="4" max="4" width="45" customWidth="1"/>
     <col min="5" max="5" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,10 +539,13 @@
         <v>37</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -541,10 +565,13 @@
         <v>11</v>
       </c>
       <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -564,10 +591,13 @@
         <v>17</v>
       </c>
       <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -587,17 +617,20 @@
         <v>22</v>
       </c>
       <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D5" t="s">
@@ -610,10 +643,13 @@
         <v>22</v>
       </c>
       <c r="H5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -633,6 +669,151 @@
         <v>22</v>
       </c>
       <c r="H6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8">
+        <v>2981</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9">
+        <v>5950</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -726,7 +907,7 @@
         <v>40656.727164351854</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" ref="E3:E9" si="0">D4-C4</f>
+        <f t="shared" ref="E4:E9" si="0">D4-C4</f>
         <v>1.1574076779652387E-5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added runs by Rodney Beede for test data
</commit_message>
<xml_diff>
--- a/docs/Test Results; 2011-04.xlsx
+++ b/docs/Test Results; 2011-04.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="113">
   <si>
     <t>Tester</t>
   </si>
@@ -47,12 +47,6 @@
     <t>linksys_FirstDictionary_!8zj39le</t>
   </si>
   <si>
-    <t>Sat Apr 23 11:25:49 MDT 2011</t>
-  </si>
-  <si>
-    <t>Sat Apr 23 11:25:54 MDT 2011</t>
-  </si>
-  <si>
     <t>Correct - No Solution</t>
   </si>
   <si>
@@ -68,30 +62,9 @@
     <t>wireless_Test_invalid_capture</t>
   </si>
   <si>
-    <t>Sat Apr 23 11:25:59 MDT 2011</t>
-  </si>
-  <si>
     <t>Job ID</t>
   </si>
   <si>
-    <t>Job_rbeede_1303579369738</t>
-  </si>
-  <si>
-    <t>Job_rbeede_1303579380995</t>
-  </si>
-  <si>
-    <t>Job_rbeede_1303579388587</t>
-  </si>
-  <si>
-    <t>Sat Apr 23 11:26:05 MDT 2011</t>
-  </si>
-  <si>
-    <t>Job_rbeede_1303579399619</t>
-  </si>
-  <si>
-    <t>Job_rbeede_1303579414118</t>
-  </si>
-  <si>
     <t>Node</t>
   </si>
   <si>
@@ -125,12 +98,6 @@
     <t>End (not sync to master)</t>
   </si>
   <si>
-    <t>Hours:Minutes:Seconds</t>
-  </si>
-  <si>
-    <t>Dist Cow - Average Run time milliseconds (no clock sync to master)</t>
-  </si>
-  <si>
     <t>Serial</t>
   </si>
   <si>
@@ -141,16 +108,258 @@
   </si>
   <si>
     <t>Serial coWPAtty run time (milliseconds)</t>
+  </si>
+  <si>
+    <t>Mast Web App - Diff (seconds)</t>
+  </si>
+  <si>
+    <t>Job_rbeede_1303593629377</t>
+  </si>
+  <si>
+    <t>Job_rbeede_1303593637402</t>
+  </si>
+  <si>
+    <t>Job_rbeede_1303593644648</t>
+  </si>
+  <si>
+    <t>Job_rbeede_1303593671797</t>
+  </si>
+  <si>
+    <t>Job_rbeede_1303593686247</t>
+  </si>
+  <si>
+    <t>Sat Apr 23 15:23:44 MDT 2011</t>
+  </si>
+  <si>
+    <t>Sat Apr 23 15:23:49 MDT 2011</t>
+  </si>
+  <si>
+    <t>Sat Apr 23 15:23:54 MDT 2011</t>
+  </si>
+  <si>
+    <t>Sat Apr 23 15:23:59 MDT 2011</t>
+  </si>
+  <si>
+    <t>Diff in milliseconds</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 705</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 701</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 702</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 729</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 703</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 747</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 682</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 740</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 778</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 706</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 785</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 707</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 795</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 708</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 805</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 837</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:02 579</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 838</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:02 586</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 839</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:02 589</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 823</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:02 566</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 846</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:02 591</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 847</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 849</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:02 605</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:01 856</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:02 600</t>
+  </si>
+  <si>
+    <t>Dist Cow - Solution Node or Longest Time - (milliseconds) (no clock sync to master)</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:06 899</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:06 900</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:06 879</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:06 903</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:06 906</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:06 905</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:07 639</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:07 654</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:07 651</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:07 634</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:07 646</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:07 641</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:07 661</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:07 672</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:11 963</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:11 982</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:11 983</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:11 964</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:11 945</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:11 965</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:11 970</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:11 992</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:11 996</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:11 986</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:11 998</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:12 8</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:17 20</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:17 25</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:17 21</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:17 26</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:17 22</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:17 27</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:17 1</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:17 6</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:17 31</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:17 32</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:17 28</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:17 33</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:17 30</t>
+  </si>
+  <si>
+    <t>2011-04-23 21:25:17 36</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="[h]:mm:ss;@"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -169,18 +378,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -195,14 +415,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,6 +437,145 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8181975" y="523875"/>
+          <a:ext cx="2371725" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Green indicates node that found the solution (if applicable)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8181975" y="4914900"/>
+          <a:ext cx="2371725" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Red indicates node took the longest when no solution was found</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -497,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -511,12 +877,13 @@
     <col min="4" max="4" width="45" customWidth="1"/>
     <col min="5" max="5" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+    <col min="8" max="8" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42" customWidth="1"/>
+    <col min="10" max="10" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,7 +894,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -536,16 +903,19 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -556,22 +926,28 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
       </c>
       <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -579,25 +955,31 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>743</v>
       </c>
       <c r="I3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -605,51 +987,63 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
         <v>39</v>
       </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>766</v>
+      </c>
       <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>15</v>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
         <v>22</v>
       </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>39</v>
-      </c>
       <c r="I5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>28</v>
+      </c>
+      <c r="J5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -657,164 +1051,173 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
       </c>
       <c r="I6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7">
+        <v>28</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7">
         <v>2</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8">
         <v>2981</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9">
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9">
         <v>5950</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>28</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+      <c r="J10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11">
+        <v>28</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11">
         <v>3</v>
       </c>
-      <c r="I11" t="s">
-        <v>12</v>
+      <c r="J11" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -825,183 +1228,755 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" style="3" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="24" style="4" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="3">
-        <v>40656.727152777778</v>
-      </c>
-      <c r="D2" s="3">
-        <v>40656.727152777778</v>
-      </c>
-      <c r="E2" s="5">
-        <f>D2-C2</f>
-        <v>0</v>
+      <c r="E1" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="7" customFormat="1">
+      <c r="A2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="9">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="6">
         <v>27</v>
-      </c>
-      <c r="C3" s="3">
-        <v>40656.727152777778</v>
-      </c>
-      <c r="D3" s="3">
-        <v>40656.727164351854</v>
-      </c>
-      <c r="E3" s="5">
-        <f>D3-C3</f>
-        <v>1.1574076779652387E-5</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="3">
-        <v>40656.727152777778</v>
-      </c>
-      <c r="D4" s="3">
-        <v>40656.727164351854</v>
-      </c>
-      <c r="E4" s="5">
-        <f t="shared" ref="E4:E9" si="0">D4-C4</f>
-        <v>1.1574076779652387E-5</v>
+      <c r="C4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="6">
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="3">
-        <v>40656.727152777778</v>
-      </c>
-      <c r="D5" s="3">
-        <v>40656.727164351854</v>
-      </c>
-      <c r="E5" s="5">
-        <f t="shared" si="0"/>
-        <v>1.1574076779652387E-5</v>
+        <v>20</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="6">
+        <f>740-682</f>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="3">
-        <v>40656.727152777778</v>
-      </c>
-      <c r="D6" s="3">
-        <v>40656.727164351854</v>
-      </c>
-      <c r="E6" s="5">
-        <f t="shared" si="0"/>
-        <v>1.1574076779652387E-5</v>
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="6">
+        <f>778-705</f>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="3">
-        <v>40656.727152777778</v>
-      </c>
-      <c r="D7" s="3">
-        <v>40656.727164351854</v>
-      </c>
-      <c r="E7" s="5">
-        <f t="shared" si="0"/>
-        <v>1.1574076779652387E-5</v>
+        <v>22</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="6">
+        <f>785-706</f>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="3">
-        <v>40656.727152777778</v>
-      </c>
-      <c r="D8" s="3">
-        <v>40656.727164351854</v>
-      </c>
-      <c r="E8" s="5">
-        <f t="shared" si="0"/>
-        <v>1.1574076779652387E-5</v>
+        <v>23</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="6">
+        <f>795-707</f>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="6">
+        <f>805-708</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="6">
+        <f>2579 - 1837</f>
+        <v>742</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="6">
+        <f>2586 - 1838</f>
+        <v>748</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="6">
+        <f>2589-1839</f>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="7" customFormat="1">
+      <c r="A13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="3">
-        <v>40656.727152777778</v>
-      </c>
-      <c r="D9" s="3">
-        <v>40656.727164351854</v>
-      </c>
-      <c r="E9" s="5">
-        <f t="shared" si="0"/>
-        <v>1.1574076779652387E-5</v>
+      <c r="B13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="9">
+        <f>2566-1823</f>
+        <v>743</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="6">
+        <f>2591-1846</f>
+        <v>745</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="6">
+        <f>2589 - 1847</f>
+        <v>742</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="6">
+        <f>2605-1849</f>
+        <v>756</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="6">
+        <f>2600-1856</f>
+        <v>744</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="6">
+        <f>7639 - 6899</f>
+        <v>740</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="6">
+        <f>7654-6899</f>
+        <v>755</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="6">
+        <f>7651-6900</f>
+        <v>751</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="6">
+        <f>7634-6879</f>
+        <v>755</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="6">
+        <f>7646-6903</f>
+        <v>743</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="6">
+        <f>7641-6903</f>
+        <v>738</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="6">
+        <f>7661-6905</f>
+        <v>756</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="7" customFormat="1">
+      <c r="A25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="9">
+        <f>7672-6906</f>
+        <v>766</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="6">
+        <f>1982-1963</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="6">
+        <f>1983-1963</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" s="6">
+        <f>1982-1964</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E29" s="6">
+        <f>1965-1945</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="11" customFormat="1">
+      <c r="A30" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="13">
+        <f>1992-1970</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E31" s="6">
+        <f>1996-1983</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="6">
+        <f>1998-1986</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E33" s="6">
+        <f>2008-1992</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E34" s="6">
+        <f>25-20</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E35" s="6">
+        <f>26-21</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E36" s="6">
+        <f>27-22</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E37" s="6">
+        <f>6-1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="11" customFormat="1">
+      <c r="A38" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="13">
+        <f>31-25</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E39" s="6">
+        <f>32-27</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E40" s="6">
+        <f>33-28</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="11" customFormat="1">
+      <c r="A41" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="E41" s="13">
+        <f>36-30</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>